<commit_message>
Updated and added more info in Biradical Visualiser Script
</commit_message>
<xml_diff>
--- a/dep/smilecodes_biradicals.xlsx
+++ b/dep/smilecodes_biradicals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/PycharmProjects/nmr_webapps/dep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482342D8-6F52-1A40-A0CB-9829452CDDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4C8086-7E76-AD4D-8D0F-A7DA622DDF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26920" xr2:uid="{1330A94C-F586-AC44-B274-89A1C0BB8025}"/>
+    <workbookView xWindow="-42540" yWindow="1580" windowWidth="51200" windowHeight="26920" xr2:uid="{1330A94C-F586-AC44-B274-89A1C0BB8025}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,12 +81,6 @@
     <t>COC(=O)N(C(=O)OC1CC2(CCC(C3=CC=CC=C3)CC2)N([O])C2(CCC(C3=CC=CC=C3)CC2)C1)C1CC2(CCC(C3=CC=CC=C3)CC2)N([O])C2(CCC(C3=CC=CC=C3)CC2)C1</t>
   </si>
   <si>
-    <t xml:space="preserve">	COCN(C(=O)OC1CC2(CCOCC2)N([O])C2(CCOCC2)C1)C1CC2(CCOCC2)N([O])C2(CCOCC2)C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	*OP(=O)(O)OC1CCC2(CC1)CC(NC(=O)C1=CC(C)(C)N([O])C1(C)C)CC1(CCC(OP(=O)(O)O)CC1)N2[O-]</t>
-  </si>
-  <si>
     <t xml:space="preserve">	CC1(C)C=C(C(=O)NC2CC3(CCC(C4=CC=CC=C4)CC3)N([O])C3(CCC(C4=CC=CC=C4)CC3)C2)C(C)(C)N1[O]</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t xml:space="preserve">	O=C(NC1CC2(CCC(O)CC2)N([O])C2(CCC(O)CC2)C1)NC1CC2(CCC(O)CC2)N([O])C2(CCC(O)CC2)C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	[K+].[O-]P(=O)([O-].[K+])OC1CCC2(CC1)CC(NC(=O)C1=CC(C)(C)N([O])C1(C)C)CC1(CCC(OP(=O)([O-].[K+])O)CC1)N2[O]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	N(CCOCOCOCOC)(C1CC2(CCOCC2)N([O])C2(CCOCC2)C1)C(OC1CC2(CCOCC2)N([O])C2(CCOCC2)C1)=O</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,15 +555,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -627,15 +627,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -643,66 +643,66 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>